<commit_message>
Adding pdf, C, xlsl files
</commit_message>
<xml_diff>
--- a/C5S7FM_0317/C5S7FMgyak6.xlsx
+++ b/C5S7FM_0317/C5S7FMgyak6.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Desktop\os orais\0317\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AA5870-5E2F-4B29-BE28-570A06CBF140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7679A31-DDE8-4EF9-A42A-B894E05EC264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11925" yWindow="540" windowWidth="16635" windowHeight="14070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.feladat" sheetId="1" r:id="rId1"/>
+    <sheet name="2.feladat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="36">
   <si>
     <t>P1</t>
   </si>
@@ -119,17 +120,35 @@
     <t>Használt időegység</t>
   </si>
   <si>
-    <t>Fenmaradt munka</t>
-  </si>
-  <si>
     <t>Gantt diagram: RR</t>
+  </si>
+  <si>
+    <t>Végrehajtási sorrend: P1 - P2 - P1 - P3 - P4 - P3 - P3</t>
+  </si>
+  <si>
+    <t>Várakozó processz</t>
+  </si>
+  <si>
+    <t>P1, P2</t>
+  </si>
+  <si>
+    <t>Gantt diagram</t>
+  </si>
+  <si>
+    <t>Várakozás:</t>
+  </si>
+  <si>
+    <t>Átlag befejezési idő:</t>
+  </si>
+  <si>
+    <t>Várakozási idők átlaga:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +165,8 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,19 +181,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,18 +237,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -540,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BU31"/>
+  <dimension ref="A1:BT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,13 +583,13 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="51" width="4.28515625" customWidth="1"/>
     <col min="52" max="73" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -576,10 +605,10 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -596,9 +625,6 @@
       <c r="F2" s="2">
         <v>20</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
         <v>1</v>
       </c>
@@ -770,8 +796,11 @@
       <c r="BS2">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -788,32 +817,33 @@
       <c r="F3" s="2">
         <v>10</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
       <c r="M3" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="7"/>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -830,24 +860,25 @@
       <c r="F4" s="2">
         <v>48</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="5"/>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="M4" t="s">
         <v>1</v>
       </c>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
       <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-    </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -856,27 +887,62 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="4"/>
       <c r="K5" t="s">
         <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5"/>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
-    </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="4"/>
+      <c r="BF5" s="4"/>
+      <c r="BG5" s="4"/>
+      <c r="BH5" s="4"/>
+      <c r="BI5" s="4"/>
+      <c r="BJ5" s="4"/>
+      <c r="BK5" s="4"/>
+      <c r="BL5" s="4"/>
+      <c r="BM5" s="4"/>
+      <c r="BN5" s="4"/>
+      <c r="BO5" s="4"/>
+      <c r="BP5" s="4"/>
+      <c r="BQ5" s="4"/>
+      <c r="BR5" s="4"/>
+      <c r="BS5" s="4"/>
+      <c r="BT5" s="4"/>
+    </row>
+    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -886,18 +952,10 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="M6" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5"/>
       <c r="AL6" s="5"/>
@@ -908,88 +966,149 @@
       <c r="AQ6" s="5"/>
       <c r="AR6" s="5"/>
       <c r="AS6" s="5"/>
-      <c r="AT6" s="6"/>
-      <c r="AU6" s="6"/>
-      <c r="AV6" s="6"/>
-      <c r="AW6" s="6"/>
-      <c r="AX6" s="6"/>
-      <c r="AY6" s="6"/>
-      <c r="AZ6" s="6"/>
-      <c r="BA6" s="6"/>
-      <c r="BB6" s="6"/>
-      <c r="BC6" s="6"/>
-      <c r="BD6" s="6"/>
-      <c r="BE6" s="6"/>
-      <c r="BF6" s="6"/>
-      <c r="BG6" s="6"/>
-      <c r="BH6" s="6"/>
-      <c r="BI6" s="6"/>
-    </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4"/>
+      <c r="AW6" s="4"/>
+      <c r="AX6" s="4"/>
+      <c r="AY6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="4"/>
+      <c r="BB6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="M7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="7"/>
-      <c r="AL7" s="7"/>
-      <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="7"/>
-      <c r="AT7" s="5"/>
-      <c r="AU7" s="5"/>
-      <c r="AV7" s="5"/>
-      <c r="AW7" s="5"/>
-      <c r="AX7" s="5"/>
-      <c r="AY7" s="5"/>
-      <c r="AZ7" s="5"/>
-      <c r="BA7" s="5"/>
-      <c r="BB7" s="5"/>
-      <c r="BC7" s="5"/>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="M8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT8" s="7"/>
-      <c r="AU8" s="7"/>
-      <c r="AV8" s="7"/>
-      <c r="AW8" s="7"/>
-      <c r="AX8" s="7"/>
-      <c r="AY8" s="7"/>
-      <c r="AZ8" s="7"/>
-      <c r="BA8" s="7"/>
-      <c r="BB8" s="7"/>
-      <c r="BC8" s="7"/>
-      <c r="BD8" s="5"/>
-      <c r="BE8" s="5"/>
-      <c r="BF8" s="5"/>
-      <c r="BG8" s="5"/>
-      <c r="BH8" s="5"/>
-      <c r="BI8" s="5"/>
-      <c r="BJ8" s="5"/>
-      <c r="BK8" s="5"/>
-      <c r="BL8" s="5"/>
-      <c r="BM8" s="5"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
+      <c r="AZ7" s="6"/>
+      <c r="BA7" s="6"/>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="6"/>
+      <c r="BE7" s="6"/>
+      <c r="BF7" s="6"/>
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6"/>
+      <c r="BI7" s="6"/>
+      <c r="BJ7" s="6"/>
+      <c r="BK7" s="6"/>
+      <c r="BL7" s="6"/>
+      <c r="BM7" s="6"/>
+      <c r="BN7" s="6"/>
+      <c r="BO7" s="6"/>
+      <c r="BP7" s="6"/>
+      <c r="BQ7" s="6"/>
+      <c r="BR7" s="6"/>
+      <c r="BS7" s="6"/>
+      <c r="BT7" s="6"/>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
+      <c r="AW8" s="6"/>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
+      <c r="BA8" s="6"/>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
+      <c r="BG8" s="6"/>
+      <c r="BH8" s="6"/>
+      <c r="BI8" s="6"/>
+      <c r="BJ8" s="6"/>
+      <c r="BK8" s="6"/>
+      <c r="BL8" s="6"/>
+      <c r="BM8" s="6"/>
       <c r="BN8" s="6"/>
       <c r="BO8" s="6"/>
       <c r="BP8" s="6"/>
       <c r="BQ8" s="6"/>
       <c r="BR8" s="6"/>
       <c r="BS8" s="6"/>
-    </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT8" s="6"/>
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1005,18 +1124,68 @@
       <c r="F9" t="s">
         <v>3</v>
       </c>
-      <c r="M9" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" s="4"/>
-      <c r="BN9" s="5"/>
-      <c r="BO9" s="5"/>
-      <c r="BP9" s="5"/>
-      <c r="BQ9" s="5"/>
-      <c r="BR9" s="5"/>
-      <c r="BS9" s="5"/>
-    </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
+      <c r="AW9" s="6"/>
+      <c r="AX9" s="6"/>
+      <c r="AY9" s="6"/>
+      <c r="AZ9" s="6"/>
+      <c r="BA9" s="6"/>
+      <c r="BB9" s="6"/>
+      <c r="BC9" s="6"/>
+      <c r="BD9" s="6"/>
+      <c r="BE9" s="6"/>
+      <c r="BF9" s="6"/>
+      <c r="BG9" s="6"/>
+      <c r="BH9" s="6"/>
+      <c r="BI9" s="6"/>
+      <c r="BJ9" s="6"/>
+      <c r="BK9" s="6"/>
+      <c r="BL9" s="6"/>
+      <c r="BM9" s="6"/>
+      <c r="BN9" s="6"/>
+      <c r="BO9" s="6"/>
+      <c r="BP9" s="6"/>
+      <c r="BQ9" s="6"/>
+      <c r="BR9" s="6"/>
+      <c r="BS9" s="6"/>
+      <c r="BT9" s="6"/>
+    </row>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1032,8 +1201,68 @@
       <c r="F10">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
+      <c r="AW10" s="6"/>
+      <c r="AX10" s="6"/>
+      <c r="AY10" s="6"/>
+      <c r="AZ10" s="6"/>
+      <c r="BA10" s="6"/>
+      <c r="BB10" s="6"/>
+      <c r="BC10" s="6"/>
+      <c r="BD10" s="6"/>
+      <c r="BE10" s="6"/>
+      <c r="BF10" s="6"/>
+      <c r="BG10" s="6"/>
+      <c r="BH10" s="6"/>
+      <c r="BI10" s="6"/>
+      <c r="BJ10" s="6"/>
+      <c r="BK10" s="6"/>
+      <c r="BL10" s="6"/>
+      <c r="BM10" s="6"/>
+      <c r="BN10" s="6"/>
+      <c r="BO10" s="6"/>
+      <c r="BP10" s="6"/>
+      <c r="BQ10" s="6"/>
+      <c r="BR10" s="6"/>
+      <c r="BS10" s="6"/>
+      <c r="BT10" s="6"/>
+    </row>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1049,8 +1278,68 @@
       <c r="F11">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="6"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
+      <c r="AV11" s="6"/>
+      <c r="AW11" s="6"/>
+      <c r="AX11" s="6"/>
+      <c r="AY11" s="6"/>
+      <c r="AZ11" s="6"/>
+      <c r="BA11" s="6"/>
+      <c r="BB11" s="6"/>
+      <c r="BC11" s="6"/>
+      <c r="BD11" s="6"/>
+      <c r="BE11" s="6"/>
+      <c r="BF11" s="6"/>
+      <c r="BG11" s="6"/>
+      <c r="BH11" s="6"/>
+      <c r="BI11" s="6"/>
+      <c r="BJ11" s="6"/>
+      <c r="BK11" s="6"/>
+      <c r="BL11" s="6"/>
+      <c r="BM11" s="6"/>
+      <c r="BN11" s="6"/>
+      <c r="BO11" s="6"/>
+      <c r="BP11" s="6"/>
+      <c r="BQ11" s="6"/>
+      <c r="BR11" s="6"/>
+      <c r="BS11" s="6"/>
+      <c r="BT11" s="6"/>
+    </row>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1073,8 +1362,199 @@
         <f>AVERAGE(B12:F12)</f>
         <v>11.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="6"/>
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="6"/>
+      <c r="AV12" s="6"/>
+      <c r="AW12" s="6"/>
+      <c r="AX12" s="6"/>
+      <c r="AY12" s="6"/>
+      <c r="AZ12" s="6"/>
+      <c r="BA12" s="6"/>
+      <c r="BB12" s="6"/>
+      <c r="BC12" s="6"/>
+      <c r="BD12" s="6"/>
+      <c r="BE12" s="6"/>
+      <c r="BF12" s="6"/>
+      <c r="BG12" s="6"/>
+      <c r="BH12" s="6"/>
+      <c r="BI12" s="6"/>
+      <c r="BJ12" s="6"/>
+      <c r="BK12" s="6"/>
+      <c r="BL12" s="6"/>
+      <c r="BM12" s="6"/>
+      <c r="BN12" s="6"/>
+      <c r="BO12" s="6"/>
+      <c r="BP12" s="6"/>
+      <c r="BQ12" s="6"/>
+      <c r="BR12" s="6"/>
+      <c r="BS12" s="6"/>
+      <c r="BT12" s="6"/>
+    </row>
+    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(B11:F11)</f>
+        <v>35.75</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="6"/>
+      <c r="AQ13" s="6"/>
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="6"/>
+      <c r="AU13" s="6"/>
+      <c r="AV13" s="6"/>
+      <c r="AW13" s="6"/>
+      <c r="AX13" s="6"/>
+      <c r="AY13" s="6"/>
+      <c r="AZ13" s="6"/>
+      <c r="BA13" s="6"/>
+      <c r="BB13" s="6"/>
+      <c r="BC13" s="6"/>
+      <c r="BD13" s="6"/>
+      <c r="BE13" s="6"/>
+      <c r="BF13" s="6"/>
+      <c r="BG13" s="6"/>
+      <c r="BH13" s="6"/>
+      <c r="BI13" s="6"/>
+      <c r="BJ13" s="6"/>
+      <c r="BK13" s="6"/>
+      <c r="BL13" s="6"/>
+      <c r="BM13" s="6"/>
+      <c r="BN13" s="6"/>
+      <c r="BO13" s="6"/>
+      <c r="BP13" s="6"/>
+      <c r="BQ13" s="6"/>
+      <c r="BR13" s="6"/>
+      <c r="BS13" s="6"/>
+      <c r="BT13" s="6"/>
+    </row>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="6"/>
+      <c r="AV14" s="6"/>
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="6"/>
+      <c r="AY14" s="6"/>
+      <c r="AZ14" s="6"/>
+      <c r="BA14" s="6"/>
+      <c r="BB14" s="6"/>
+      <c r="BC14" s="6"/>
+      <c r="BD14" s="6"/>
+      <c r="BE14" s="6"/>
+      <c r="BF14" s="6"/>
+      <c r="BG14" s="6"/>
+      <c r="BH14" s="6"/>
+      <c r="BI14" s="6"/>
+      <c r="BJ14" s="6"/>
+      <c r="BK14" s="6"/>
+      <c r="BL14" s="6"/>
+      <c r="BM14" s="6"/>
+      <c r="BN14" s="6"/>
+      <c r="BO14" s="6"/>
+      <c r="BP14" s="6"/>
+      <c r="BQ14" s="6"/>
+      <c r="BR14" s="6"/>
+      <c r="BS14" s="6"/>
+      <c r="BT14" s="6"/>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1091,7 +1571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1165,6 +1645,13 @@
       <c r="F19" t="s">
         <v>16</v>
       </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19">
+        <f>AVERAGE(B17:F17)</f>
+        <v>31.75</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1269,22 +1756,22 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F26" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G26" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H26" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1292,25 +1779,25 @@
         <v>7</v>
       </c>
       <c r="B27" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D27" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E27" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F27" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G27" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H27" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1367,7 +1854,7 @@
       <c r="J29" t="s">
         <v>26</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="12">
         <f>AVERAGE(B28:H28)</f>
         <v>5.8571428571428568</v>
       </c>
@@ -1396,6 +1883,13 @@
       </c>
       <c r="H30" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="12">
+        <f>AVERAGE(B27:H27)</f>
+        <v>33.285714285714285</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,8 +1900,704 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E16B753-D2B7-4EE5-AF2C-653F4985F956}">
+  <dimension ref="A1:BY25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="77" width="4.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
+        <v>7</v>
+      </c>
+      <c r="D2" s="15">
+        <v>11</v>
+      </c>
+      <c r="E2" s="16">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2">
+        <v>11</v>
+      </c>
+      <c r="U2">
+        <v>12</v>
+      </c>
+      <c r="V2">
+        <v>13</v>
+      </c>
+      <c r="W2">
+        <v>14</v>
+      </c>
+      <c r="X2">
+        <v>15</v>
+      </c>
+      <c r="Y2">
+        <v>16</v>
+      </c>
+      <c r="Z2">
+        <v>17</v>
+      </c>
+      <c r="AA2">
+        <v>18</v>
+      </c>
+      <c r="AB2">
+        <v>19</v>
+      </c>
+      <c r="AC2">
+        <v>20</v>
+      </c>
+      <c r="AD2">
+        <v>21</v>
+      </c>
+      <c r="AE2">
+        <v>22</v>
+      </c>
+      <c r="AF2">
+        <v>23</v>
+      </c>
+      <c r="AG2">
+        <v>24</v>
+      </c>
+      <c r="AH2">
+        <v>25</v>
+      </c>
+      <c r="AI2">
+        <v>26</v>
+      </c>
+      <c r="AJ2">
+        <v>27</v>
+      </c>
+      <c r="AK2">
+        <v>28</v>
+      </c>
+      <c r="AL2">
+        <v>29</v>
+      </c>
+      <c r="AM2">
+        <v>30</v>
+      </c>
+      <c r="AN2">
+        <v>31</v>
+      </c>
+      <c r="AO2">
+        <v>32</v>
+      </c>
+      <c r="AP2">
+        <v>33</v>
+      </c>
+      <c r="AQ2">
+        <v>34</v>
+      </c>
+      <c r="AR2">
+        <v>35</v>
+      </c>
+      <c r="AS2">
+        <v>36</v>
+      </c>
+      <c r="AT2">
+        <v>37</v>
+      </c>
+      <c r="AU2">
+        <v>38</v>
+      </c>
+      <c r="AV2">
+        <v>39</v>
+      </c>
+      <c r="AW2">
+        <v>40</v>
+      </c>
+      <c r="AX2">
+        <v>41</v>
+      </c>
+      <c r="AY2">
+        <v>42</v>
+      </c>
+      <c r="AZ2">
+        <v>43</v>
+      </c>
+      <c r="BA2">
+        <v>44</v>
+      </c>
+      <c r="BB2">
+        <v>45</v>
+      </c>
+      <c r="BC2">
+        <v>46</v>
+      </c>
+      <c r="BD2">
+        <v>47</v>
+      </c>
+      <c r="BE2">
+        <v>48</v>
+      </c>
+      <c r="BF2">
+        <v>49</v>
+      </c>
+      <c r="BG2">
+        <v>50</v>
+      </c>
+      <c r="BH2">
+        <v>51</v>
+      </c>
+      <c r="BI2">
+        <v>52</v>
+      </c>
+      <c r="BJ2">
+        <v>53</v>
+      </c>
+      <c r="BK2">
+        <v>54</v>
+      </c>
+      <c r="BL2">
+        <v>55</v>
+      </c>
+      <c r="BM2">
+        <v>56</v>
+      </c>
+      <c r="BN2">
+        <v>57</v>
+      </c>
+      <c r="BO2">
+        <v>58</v>
+      </c>
+      <c r="BP2">
+        <v>59</v>
+      </c>
+      <c r="BQ2">
+        <v>60</v>
+      </c>
+      <c r="BR2">
+        <v>61</v>
+      </c>
+      <c r="BS2">
+        <v>62</v>
+      </c>
+      <c r="BT2">
+        <v>63</v>
+      </c>
+      <c r="BU2">
+        <v>64</v>
+      </c>
+      <c r="BV2">
+        <v>65</v>
+      </c>
+      <c r="BW2">
+        <v>66</v>
+      </c>
+      <c r="BX2">
+        <v>67</v>
+      </c>
+      <c r="BY2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14">
+        <v>8</v>
+      </c>
+      <c r="D3" s="15">
+        <v>36</v>
+      </c>
+      <c r="E3" s="16">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+    </row>
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13">
+        <v>22</v>
+      </c>
+      <c r="C4" s="14">
+        <v>18</v>
+      </c>
+      <c r="D4" s="15">
+        <v>68</v>
+      </c>
+      <c r="E4" s="16">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+    </row>
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="13">
+        <v>8</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3</v>
+      </c>
+      <c r="D5" s="15">
+        <v>21</v>
+      </c>
+      <c r="E5" s="16">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="10"/>
+      <c r="BC5" s="10"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="10"/>
+      <c r="BF5" s="10"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10"/>
+      <c r="BL5" s="10"/>
+      <c r="BM5" s="10"/>
+      <c r="BN5" s="10"/>
+      <c r="BO5" s="10"/>
+      <c r="BP5" s="10"/>
+      <c r="BQ5" s="10"/>
+      <c r="BR5" s="10"/>
+      <c r="BS5" s="10"/>
+      <c r="BT5" s="10"/>
+      <c r="BU5" s="10"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="10"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="10"/>
+    </row>
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="11"/>
+    </row>
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9">
+        <v>8</v>
+      </c>
+      <c r="D13" s="9">
+        <v>10</v>
+      </c>
+      <c r="E13" s="9">
+        <v>18</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8">
+        <v>8</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10">
+        <v>36</v>
+      </c>
+      <c r="D15" s="10">
+        <v>22</v>
+      </c>
+      <c r="E15" s="10">
+        <v>32</v>
+      </c>
+      <c r="F15" s="10">
+        <v>11</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11">
+        <v>10</v>
+      </c>
+      <c r="D16" s="11">
+        <v>32</v>
+      </c>
+      <c r="E16" s="11">
+        <v>42</v>
+      </c>
+      <c r="F16" s="11">
+        <v>12</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="10">
+        <v>32</v>
+      </c>
+      <c r="C17" s="10">
+        <v>26</v>
+      </c>
+      <c r="D17" s="10">
+        <v>42</v>
+      </c>
+      <c r="E17" s="10">
+        <v>52</v>
+      </c>
+      <c r="F17" s="10">
+        <v>10</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="10">
+        <v>52</v>
+      </c>
+      <c r="C18" s="10">
+        <v>16</v>
+      </c>
+      <c r="D18" s="10">
+        <v>52</v>
+      </c>
+      <c r="E18" s="10">
+        <v>62</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10">
+        <v>62</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6</v>
+      </c>
+      <c r="D19" s="10">
+        <v>62</v>
+      </c>
+      <c r="E19" s="10">
+        <v>68</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25">
+        <f>AVERAGE(F12:F19)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>